<commit_message>
end of manual testing
</commit_message>
<xml_diff>
--- a/etudes_de_cas.xlsx
+++ b/etudes_de_cas.xlsx
@@ -492,7 +492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E5"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,31 @@
         </is>
       </c>
       <c r="E5" s="13" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="inlineStr">
+        <is>
+          <t>WESTERN, BOTTE SANTIAG VELOURS TAUPE</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>Femme</t>
+        </is>
+      </c>
+      <c r="C6" s="10" t="inlineStr">
+        <is>
+          <t>Shoes</t>
+        </is>
+      </c>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>https://www.labottegardiane.com/products/western-paris-botte-santiag-velours-taupe#</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -607,7 +632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W44"/>
+  <dimension ref="A1:W64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,7 +640,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
@@ -2777,6 +2802,7 @@
         </is>
       </c>
     </row>
+    <row r="36"/>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
@@ -2797,6 +2823,7 @@
         </is>
       </c>
     </row>
+    <row r="38"/>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
@@ -3217,6 +3244,1388 @@
       <c r="N44" s="6" t="inlineStr">
         <is>
           <t>32.1 cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="45"/>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>Guide de taille</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C46" s="3" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="D46" s="11" t="inlineStr">
+        <is>
+          <t>https://www.labottegardiane.com/products/western-paris-botte-santiag-velours-taupe#</t>
+        </is>
+      </c>
+    </row>
+    <row r="47"/>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>Systemes metriques</t>
+        </is>
+      </c>
+      <c r="B48" s="5" t="inlineStr"/>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 1</t>
+        </is>
+      </c>
+      <c r="D48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 2</t>
+        </is>
+      </c>
+      <c r="E48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 3</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 4</t>
+        </is>
+      </c>
+      <c r="G48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 5</t>
+        </is>
+      </c>
+      <c r="H48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 6</t>
+        </is>
+      </c>
+      <c r="I48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 7</t>
+        </is>
+      </c>
+      <c r="J48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 8</t>
+        </is>
+      </c>
+      <c r="K48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 9</t>
+        </is>
+      </c>
+      <c r="L48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 10</t>
+        </is>
+      </c>
+      <c r="M48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 11</t>
+        </is>
+      </c>
+      <c r="N48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 12</t>
+        </is>
+      </c>
+      <c r="O48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 13</t>
+        </is>
+      </c>
+      <c r="P48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 14</t>
+        </is>
+      </c>
+      <c r="Q48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 15</t>
+        </is>
+      </c>
+      <c r="R48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 16</t>
+        </is>
+      </c>
+      <c r="S48" s="1" t="inlineStr">
+        <is>
+          <t>Taille 17</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>La Bottega Gardiane</t>
+        </is>
+      </c>
+      <c r="B49" s="7" t="inlineStr">
+        <is>
+          <t>La Bottega Gardiane</t>
+        </is>
+      </c>
+      <c r="C49" s="6" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="D49" s="6" t="inlineStr">
+        <is>
+          <t>39.5</t>
+        </is>
+      </c>
+      <c r="E49" s="6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="F49" s="6" t="inlineStr">
+        <is>
+          <t>40.5</t>
+        </is>
+      </c>
+      <c r="G49" s="6" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="H49" s="6" t="inlineStr">
+        <is>
+          <t>41.5</t>
+        </is>
+      </c>
+      <c r="I49" s="6" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="J49" s="6" t="inlineStr">
+        <is>
+          <t>42.5</t>
+        </is>
+      </c>
+      <c r="K49" s="6" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="L49" s="6" t="inlineStr">
+        <is>
+          <t>43.5</t>
+        </is>
+      </c>
+      <c r="M49" s="6" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="N49" s="6" t="inlineStr">
+        <is>
+          <t>44.5</t>
+        </is>
+      </c>
+      <c r="O49" s="6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="P49" s="6" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="Q49" s="6" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="R49" s="6" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="S49" s="6" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="B50" s="7" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="C50" s="6" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="D50" s="6" t="inlineStr">
+        <is>
+          <t>39.5</t>
+        </is>
+      </c>
+      <c r="E50" s="6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="F50" s="6" t="inlineStr">
+        <is>
+          <t>40.5</t>
+        </is>
+      </c>
+      <c r="G50" s="6" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="H50" s="6" t="inlineStr">
+        <is>
+          <t>41.5</t>
+        </is>
+      </c>
+      <c r="I50" s="6" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="J50" s="6" t="inlineStr">
+        <is>
+          <t>42.5</t>
+        </is>
+      </c>
+      <c r="K50" s="6" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="L50" s="6" t="inlineStr">
+        <is>
+          <t>43.5</t>
+        </is>
+      </c>
+      <c r="M50" s="6" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="N50" s="6" t="inlineStr">
+        <is>
+          <t>44.5</t>
+        </is>
+      </c>
+      <c r="O50" s="6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="P50" s="6" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="Q50" s="6" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="R50" s="6" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="S50" s="6" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="inlineStr">
+        <is>
+          <t>Royaume-Uni</t>
+        </is>
+      </c>
+      <c r="B51" s="7" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="C51" s="6" t="inlineStr">
+        <is>
+          <t>5.5</t>
+        </is>
+      </c>
+      <c r="D51" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E51" s="6" t="inlineStr">
+        <is>
+          <t>6.5</t>
+        </is>
+      </c>
+      <c r="F51" s="6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G51" s="6" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
+      </c>
+      <c r="H51" s="6" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
+      </c>
+      <c r="I51" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="J51" s="6" t="inlineStr">
+        <is>
+          <t>8.5</t>
+        </is>
+      </c>
+      <c r="K51" s="6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="L51" s="6" t="inlineStr">
+        <is>
+          <t>9.5</t>
+        </is>
+      </c>
+      <c r="M51" s="6" t="inlineStr">
+        <is>
+          <t>9.5</t>
+        </is>
+      </c>
+      <c r="N51" s="6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="O51" s="6" t="inlineStr">
+        <is>
+          <t>10.5</t>
+        </is>
+      </c>
+      <c r="P51" s="6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="Q51" s="6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="R51" s="6" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="S51" s="6" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="inlineStr">
+        <is>
+          <t>Etats-Unis</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="C52" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D52" s="6" t="inlineStr">
+        <is>
+          <t>6.5</t>
+        </is>
+      </c>
+      <c r="E52" s="6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F52" s="6" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
+      </c>
+      <c r="G52" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H52" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I52" s="6" t="inlineStr">
+        <is>
+          <t>8.5</t>
+        </is>
+      </c>
+      <c r="J52" s="6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="K52" s="6" t="inlineStr">
+        <is>
+          <t>9.5</t>
+        </is>
+      </c>
+      <c r="L52" s="6" t="inlineStr">
+        <is>
+          <t>9.5</t>
+        </is>
+      </c>
+      <c r="M52" s="6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="N52" s="6" t="inlineStr">
+        <is>
+          <t>10.5</t>
+        </is>
+      </c>
+      <c r="O52" s="6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="P52" s="6" t="inlineStr">
+        <is>
+          <t>11.5</t>
+        </is>
+      </c>
+      <c r="Q52" s="6" t="inlineStr">
+        <is>
+          <t>12.5</t>
+        </is>
+      </c>
+      <c r="R52" s="6" t="inlineStr">
+        <is>
+          <t>13.5</t>
+        </is>
+      </c>
+      <c r="S52" s="6" t="inlineStr">
+        <is>
+          <t>14.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>Italie</t>
+        </is>
+      </c>
+      <c r="B53" s="7" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="C53" s="6" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>38.5</t>
+        </is>
+      </c>
+      <c r="E53" s="6" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="F53" s="6" t="inlineStr">
+        <is>
+          <t>39.5</t>
+        </is>
+      </c>
+      <c r="G53" s="6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="H53" s="6" t="inlineStr">
+        <is>
+          <t>40.5</t>
+        </is>
+      </c>
+      <c r="I53" s="6" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="J53" s="6" t="inlineStr">
+        <is>
+          <t>41.5</t>
+        </is>
+      </c>
+      <c r="K53" s="6" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="L53" s="6" t="inlineStr">
+        <is>
+          <t>42.5</t>
+        </is>
+      </c>
+      <c r="M53" s="6" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="N53" s="6" t="inlineStr">
+        <is>
+          <t>43.5</t>
+        </is>
+      </c>
+      <c r="O53" s="6" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="P53" s="6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="Q53" s="6" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="R53" s="6" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="S53" s="6" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6" t="inlineStr">
+        <is>
+          <t>Longueur pied</t>
+        </is>
+      </c>
+      <c r="C54" s="6" t="inlineStr">
+        <is>
+          <t>25 cm</t>
+        </is>
+      </c>
+      <c r="D54" s="6" t="inlineStr">
+        <is>
+          <t>25.4 cm</t>
+        </is>
+      </c>
+      <c r="E54" s="6" t="inlineStr">
+        <is>
+          <t>25.7 cm</t>
+        </is>
+      </c>
+      <c r="F54" s="6" t="inlineStr">
+        <is>
+          <t>26 cm</t>
+        </is>
+      </c>
+      <c r="G54" s="6" t="inlineStr">
+        <is>
+          <t>26.4 cm</t>
+        </is>
+      </c>
+      <c r="H54" s="6" t="inlineStr">
+        <is>
+          <t>26.4 cm</t>
+        </is>
+      </c>
+      <c r="I54" s="6" t="inlineStr">
+        <is>
+          <t>26.7 cm</t>
+        </is>
+      </c>
+      <c r="J54" s="6" t="inlineStr">
+        <is>
+          <t>27.4 cm</t>
+        </is>
+      </c>
+      <c r="K54" s="6" t="inlineStr">
+        <is>
+          <t>27.7 cm</t>
+        </is>
+      </c>
+      <c r="L54" s="6" t="inlineStr">
+        <is>
+          <t>28 cm</t>
+        </is>
+      </c>
+      <c r="M54" s="6" t="inlineStr">
+        <is>
+          <t>28.4 cm</t>
+        </is>
+      </c>
+      <c r="N54" s="6" t="inlineStr">
+        <is>
+          <t>28.7 cm</t>
+        </is>
+      </c>
+      <c r="O54" s="6" t="inlineStr">
+        <is>
+          <t>29 cm</t>
+        </is>
+      </c>
+      <c r="P54" s="6" t="inlineStr">
+        <is>
+          <t>29.7 cm</t>
+        </is>
+      </c>
+      <c r="Q54" s="6" t="inlineStr">
+        <is>
+          <t>30.4 cm</t>
+        </is>
+      </c>
+      <c r="R54" s="6" t="inlineStr">
+        <is>
+          <t>31 cm</t>
+        </is>
+      </c>
+      <c r="S54" s="6" t="inlineStr">
+        <is>
+          <t>31.7 cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>Guide de taille</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C56" s="3" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="D56" s="11" t="inlineStr">
+        <is>
+          <t>https://www.labottegardiane.com/products/western-paris-botte-santiag-velours-taupe#</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>Systemes metriques</t>
+        </is>
+      </c>
+      <c r="B58" s="5" t="inlineStr"/>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 1</t>
+        </is>
+      </c>
+      <c r="D58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 2</t>
+        </is>
+      </c>
+      <c r="E58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 3</t>
+        </is>
+      </c>
+      <c r="F58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 4</t>
+        </is>
+      </c>
+      <c r="G58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 5</t>
+        </is>
+      </c>
+      <c r="H58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 6</t>
+        </is>
+      </c>
+      <c r="I58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 7</t>
+        </is>
+      </c>
+      <c r="J58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 8</t>
+        </is>
+      </c>
+      <c r="K58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 9</t>
+        </is>
+      </c>
+      <c r="L58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 10</t>
+        </is>
+      </c>
+      <c r="M58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 11</t>
+        </is>
+      </c>
+      <c r="N58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 12</t>
+        </is>
+      </c>
+      <c r="O58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 13</t>
+        </is>
+      </c>
+      <c r="P58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 14</t>
+        </is>
+      </c>
+      <c r="Q58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 15</t>
+        </is>
+      </c>
+      <c r="R58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 16</t>
+        </is>
+      </c>
+      <c r="S58" s="1" t="inlineStr">
+        <is>
+          <t>Taille 17</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="inlineStr">
+        <is>
+          <t>La Bottega Gardiane</t>
+        </is>
+      </c>
+      <c r="B59" s="7" t="inlineStr">
+        <is>
+          <t>La Bottega Gardiane</t>
+        </is>
+      </c>
+      <c r="C59" s="6" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>39.5</t>
+        </is>
+      </c>
+      <c r="E59" s="6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="F59" s="6" t="inlineStr">
+        <is>
+          <t>40.5</t>
+        </is>
+      </c>
+      <c r="G59" s="6" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="H59" s="6" t="inlineStr">
+        <is>
+          <t>41.5</t>
+        </is>
+      </c>
+      <c r="I59" s="6" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="J59" s="6" t="inlineStr">
+        <is>
+          <t>42.5</t>
+        </is>
+      </c>
+      <c r="K59" s="6" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="L59" s="6" t="inlineStr">
+        <is>
+          <t>43.5</t>
+        </is>
+      </c>
+      <c r="M59" s="6" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="N59" s="6" t="inlineStr">
+        <is>
+          <t>44.5</t>
+        </is>
+      </c>
+      <c r="O59" s="6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="P59" s="6" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="Q59" s="6" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="R59" s="6" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="S59" s="6" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="6" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="B60" s="7" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="C60" s="6" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="D60" s="6" t="inlineStr">
+        <is>
+          <t>39.5</t>
+        </is>
+      </c>
+      <c r="E60" s="6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="F60" s="6" t="inlineStr">
+        <is>
+          <t>40.5</t>
+        </is>
+      </c>
+      <c r="G60" s="6" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="H60" s="6" t="inlineStr">
+        <is>
+          <t>41.5</t>
+        </is>
+      </c>
+      <c r="I60" s="6" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="J60" s="6" t="inlineStr">
+        <is>
+          <t>42.5</t>
+        </is>
+      </c>
+      <c r="K60" s="6" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="L60" s="6" t="inlineStr">
+        <is>
+          <t>43.5</t>
+        </is>
+      </c>
+      <c r="M60" s="6" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="N60" s="6" t="inlineStr">
+        <is>
+          <t>44.5</t>
+        </is>
+      </c>
+      <c r="O60" s="6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="P60" s="6" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="Q60" s="6" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="R60" s="6" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="S60" s="6" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="inlineStr">
+        <is>
+          <t>Royaume-Uni</t>
+        </is>
+      </c>
+      <c r="B61" s="7" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>5.5</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E61" s="6" t="inlineStr">
+        <is>
+          <t>6.5</t>
+        </is>
+      </c>
+      <c r="F61" s="6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G61" s="6" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
+      </c>
+      <c r="H61" s="6" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
+      </c>
+      <c r="I61" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="J61" s="6" t="inlineStr">
+        <is>
+          <t>8.5</t>
+        </is>
+      </c>
+      <c r="K61" s="6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="L61" s="6" t="inlineStr">
+        <is>
+          <t>9.5</t>
+        </is>
+      </c>
+      <c r="M61" s="6" t="inlineStr">
+        <is>
+          <t>9.5</t>
+        </is>
+      </c>
+      <c r="N61" s="6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="O61" s="6" t="inlineStr">
+        <is>
+          <t>10.5</t>
+        </is>
+      </c>
+      <c r="P61" s="6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="Q61" s="6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="R61" s="6" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="S61" s="6" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="6" t="inlineStr">
+        <is>
+          <t>Etats-Unis</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="C62" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D62" s="6" t="inlineStr">
+        <is>
+          <t>6.5</t>
+        </is>
+      </c>
+      <c r="E62" s="6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F62" s="6" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
+      </c>
+      <c r="G62" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H62" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I62" s="6" t="inlineStr">
+        <is>
+          <t>8.5</t>
+        </is>
+      </c>
+      <c r="J62" s="6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="K62" s="6" t="inlineStr">
+        <is>
+          <t>9.5</t>
+        </is>
+      </c>
+      <c r="L62" s="6" t="inlineStr">
+        <is>
+          <t>9.5</t>
+        </is>
+      </c>
+      <c r="M62" s="6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="N62" s="6" t="inlineStr">
+        <is>
+          <t>10.5</t>
+        </is>
+      </c>
+      <c r="O62" s="6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="P62" s="6" t="inlineStr">
+        <is>
+          <t>11.5</t>
+        </is>
+      </c>
+      <c r="Q62" s="6" t="inlineStr">
+        <is>
+          <t>12.5</t>
+        </is>
+      </c>
+      <c r="R62" s="6" t="inlineStr">
+        <is>
+          <t>13.5</t>
+        </is>
+      </c>
+      <c r="S62" s="6" t="inlineStr">
+        <is>
+          <t>14.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="inlineStr">
+        <is>
+          <t>Italie</t>
+        </is>
+      </c>
+      <c r="B63" s="7" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="C63" s="6" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D63" s="6" t="inlineStr">
+        <is>
+          <t>38.5</t>
+        </is>
+      </c>
+      <c r="E63" s="6" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="F63" s="6" t="inlineStr">
+        <is>
+          <t>39.5</t>
+        </is>
+      </c>
+      <c r="G63" s="6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="H63" s="6" t="inlineStr">
+        <is>
+          <t>40.5</t>
+        </is>
+      </c>
+      <c r="I63" s="6" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="J63" s="6" t="inlineStr">
+        <is>
+          <t>41.5</t>
+        </is>
+      </c>
+      <c r="K63" s="6" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="L63" s="6" t="inlineStr">
+        <is>
+          <t>42.5</t>
+        </is>
+      </c>
+      <c r="M63" s="6" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="N63" s="6" t="inlineStr">
+        <is>
+          <t>43.5</t>
+        </is>
+      </c>
+      <c r="O63" s="6" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="P63" s="6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="Q63" s="6" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="R63" s="6" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="S63" s="6" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="6" t="inlineStr">
+        <is>
+          <t>Longueur pied</t>
+        </is>
+      </c>
+      <c r="C64" s="6" t="inlineStr">
+        <is>
+          <t>25 cm</t>
+        </is>
+      </c>
+      <c r="D64" s="6" t="inlineStr">
+        <is>
+          <t>25.4 cm</t>
+        </is>
+      </c>
+      <c r="E64" s="6" t="inlineStr">
+        <is>
+          <t>25.7 cm</t>
+        </is>
+      </c>
+      <c r="F64" s="6" t="inlineStr">
+        <is>
+          <t>26 cm</t>
+        </is>
+      </c>
+      <c r="G64" s="6" t="inlineStr">
+        <is>
+          <t>26.4 cm</t>
+        </is>
+      </c>
+      <c r="H64" s="6" t="inlineStr">
+        <is>
+          <t>26.4 cm</t>
+        </is>
+      </c>
+      <c r="I64" s="6" t="inlineStr">
+        <is>
+          <t>26.7 cm</t>
+        </is>
+      </c>
+      <c r="J64" s="6" t="inlineStr">
+        <is>
+          <t>27.4 cm</t>
+        </is>
+      </c>
+      <c r="K64" s="6" t="inlineStr">
+        <is>
+          <t>27.7 cm</t>
+        </is>
+      </c>
+      <c r="L64" s="6" t="inlineStr">
+        <is>
+          <t>28 cm</t>
+        </is>
+      </c>
+      <c r="M64" s="6" t="inlineStr">
+        <is>
+          <t>28.4 cm</t>
+        </is>
+      </c>
+      <c r="N64" s="6" t="inlineStr">
+        <is>
+          <t>28.7 cm</t>
+        </is>
+      </c>
+      <c r="O64" s="6" t="inlineStr">
+        <is>
+          <t>29 cm</t>
+        </is>
+      </c>
+      <c r="P64" s="6" t="inlineStr">
+        <is>
+          <t>29.7 cm</t>
+        </is>
+      </c>
+      <c r="Q64" s="6" t="inlineStr">
+        <is>
+          <t>30.4 cm</t>
+        </is>
+      </c>
+      <c r="R64" s="6" t="inlineStr">
+        <is>
+          <t>31 cm</t>
+        </is>
+      </c>
+      <c r="S64" s="6" t="inlineStr">
+        <is>
+          <t>31.7 cm</t>
         </is>
       </c>
     </row>

</xml_diff>